<commit_message>
Updated localizations a bit
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,12 +23,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
-  <si>
-    <t xml:space="preserve">menu.start_game</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start Game</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+  <si>
+    <t xml:space="preserve">menu.new_run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Run</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menu.continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continue</t>
   </si>
   <si>
     <t xml:space="preserve">menu.settings</t>
@@ -37,25 +43,73 @@
     <t xml:space="preserve">Settings</t>
   </si>
   <si>
-    <t xml:space="preserve">menu.about</t>
-  </si>
-  <si>
-    <t xml:space="preserve">About</t>
-  </si>
-  <si>
-    <t xml:space="preserve">menu.exit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start het spel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Starta spelet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ξεκίνα το παιχνίδι</t>
+    <t xml:space="preserve">menu.database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menu.credits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Credits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menu.quit_game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quit Game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nieuw Spel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doorgaan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instellingen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Databank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spel Afsluiten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nytt spel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fortsätta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inställningar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Databas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krediter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avsluta spelet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Νέο παιχνίδι</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Να συνεχίσει</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ρυθμίσεις</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Βάση δεδομένων</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Πιστώσεις</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Κλείστε το παιχνίδι</t>
   </si>
 </sst>
 </file>
@@ -157,13 +211,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.47"/>
   </cols>
@@ -176,11 +230,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -192,12 +246,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -216,13 +286,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.32"/>
@@ -234,7 +304,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -253,13 +363,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.8"/>
@@ -271,7 +381,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -290,13 +440,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:B"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.12"/>
@@ -308,7 +458,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more texts to test localization
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Nederlands" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Svenska" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Ελληνικά" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Svenska" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Ελληνικά" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Nederlands" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
   <si>
     <t xml:space="preserve">menu.new_run</t>
   </si>
@@ -109,6 +109,87 @@
     <t xml:space="preserve">Select primary and secondary weapon</t>
   </si>
   <si>
+    <t xml:space="preserve">Nytt spel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fortsätta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inställningar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Databas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Krediter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avsluta spelet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Börja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Svårighet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En promenad i ödemarkerna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jogga med monster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frukta mig fula odjur!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jag är... Skötaren</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Välj Tecken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Välj primärt och sekundärt vapen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Νέο παιχνίδι</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Να συνεχίσει</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ρυθμίσεις</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Βάση δεδομένων</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Πιστώσεις</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Κλείστε το παιχνίδι</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Αρχίζουν</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Δυσκολία</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Μια βόλτα στις ερημιές</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Τζόκινγκ με τέρατα</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Είμαι… Ο οδοκαθαριστής</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Επιλέξτε Χαρακτήρας</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Επιλέξτε κύριο και δευτερεύον όπλο</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nieuw Spel</t>
   </si>
   <si>
@@ -124,40 +205,28 @@
     <t xml:space="preserve">Spel Afsluiten</t>
   </si>
   <si>
-    <t xml:space="preserve">Nytt spel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fortsätta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inställningar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Databas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Krediter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Avsluta spelet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Νέο παιχνίδι</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Να συνεχίσει</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ρυθμίσεις</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Βάση δεδομένων</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Πιστώσεις</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Κλείστε το παιχνίδι</t>
+    <t xml:space="preserve">Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moeilijkheidsgraad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Een wandeling door de woestenijen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joggen met monsters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vrees me vuile beesten!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ik ben... de Allesvreter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selecteer Karakter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Selecteer primair en secundair wapen</t>
   </si>
 </sst>
 </file>
@@ -261,13 +330,13 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -398,16 +467,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.8"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="10.5"/>
   </cols>
   <sheetData>
@@ -448,7 +517,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -456,7 +525,71 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -475,16 +608,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="H37" activeCellId="1" sqref="A1:B14 H37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.12"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="10.5"/>
   </cols>
   <sheetData>
@@ -493,7 +626,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -501,44 +634,104 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>35</v>
+      <c r="B3" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>36</v>
+      <c r="B4" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>37</v>
+      <c r="B5" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>38</v>
+      <c r="B6" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -556,25 +749,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="10.5"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,48 +770,112 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>41</v>
+      <c r="B3" s="1" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>42</v>
+      <c r="B4" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>43</v>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>44</v>
+      <c r="B6" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on texts in scenes
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -67,7 +67,7 @@
     <t xml:space="preserve">Begin</t>
   </si>
   <si>
-    <t xml:space="preserve">newrun.difficulty</t>
+    <t xml:space="preserve">newrun.title_difficulty</t>
   </si>
   <si>
     <t xml:space="preserve">Difficulty</t>
@@ -97,16 +97,16 @@
     <t xml:space="preserve">I Am… The Scavenger</t>
   </si>
   <si>
-    <t xml:space="preserve">newrun.select_character</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select Character</t>
-  </si>
-  <si>
-    <t xml:space="preserve">newrun.select_weapons</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select primary and secondary weapon</t>
+    <t xml:space="preserve">newrun.title_character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Character</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newrun.title_specializations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specializations</t>
   </si>
   <si>
     <t xml:space="preserve">Nytt spel</t>
@@ -145,10 +145,10 @@
     <t xml:space="preserve">Jag är... Skötaren</t>
   </si>
   <si>
-    <t xml:space="preserve">Välj Tecken</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Välj primärt och sekundärt vapen</t>
+    <t xml:space="preserve">Karaktär</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specialiteter</t>
   </si>
   <si>
     <t xml:space="preserve">Νέο παιχνίδι</t>
@@ -187,10 +187,10 @@
     <t xml:space="preserve">Είμαι… Ο οδοκαθαριστής</t>
   </si>
   <si>
-    <t xml:space="preserve">Επιλέξτε Χαρακτήρας</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Επιλέξτε κύριο και δευτερεύον όπλο</t>
+    <t xml:space="preserve">Χαρακτήρας</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ειδικότητες</t>
   </si>
   <si>
     <t xml:space="preserve">Nieuw Spel</t>
@@ -226,10 +226,10 @@
     <t xml:space="preserve">Ik ben... de Allesvreter</t>
   </si>
   <si>
-    <t xml:space="preserve">Selecteer Karakter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Selecteer primair en secundair wapen</t>
+    <t xml:space="preserve">Karakter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specialiteiten</t>
   </si>
 </sst>
 </file>
@@ -239,7 +239,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -261,6 +261,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -305,13 +311,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -337,9 +351,9 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -470,13 +484,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.8"/>
@@ -532,7 +546,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
@@ -540,7 +554,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -583,17 +597,19 @@
       <c r="A13" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="0" t="s">
         <v>40</v>
       </c>
+      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="0" t="s">
         <v>41</v>
       </c>
+      <c r="AMJ14" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -611,22 +627,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.51953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.12"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>42</v>
@@ -724,17 +740,19 @@
       <c r="A13" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="3" t="s">
         <v>54</v>
       </c>
+      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="AMJ14" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -755,10 +773,13 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.66"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Worked on mission briefing scene
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
   <si>
     <t xml:space="preserve">menu.new_run</t>
   </si>
@@ -97,6 +97,108 @@
     <t xml:space="preserve">I Am… The Scavenger</t>
   </si>
   <si>
+    <t xml:space="preserve">newrun.difficulty1.tagline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No modifiers. A typical Tuesday.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">newrun.difficulty2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.tagline</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Some people like challenges.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">newrun.difficulty3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.tagline</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Life will get tough.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">newrun.difficulty4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">.tagline</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Only the strongest will survive.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newrun.difficulty1.digit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newrun.difficulty2.digit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newrun.difficulty3.digit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newrun.difficulty4.digit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
     <t xml:space="preserve">newrun.title_character</t>
   </si>
   <si>
@@ -107,6 +209,18 @@
   </si>
   <si>
     <t xml:space="preserve">Specializations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character1.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mac “Maggot” the Hired Gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">character1.description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maggot uses decoys to confuse his opponents and can earn money faster than anyone.</t>
   </si>
   <si>
     <t xml:space="preserve">Nytt spel</t>
@@ -311,16 +425,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -345,13 +455,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:AMJ24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.7"/>
   </cols>
@@ -372,7 +482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
@@ -388,7 +498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
@@ -396,7 +506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>10</v>
       </c>
@@ -412,7 +522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>14</v>
       </c>
@@ -420,7 +530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>16</v>
       </c>
@@ -428,7 +538,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>18</v>
       </c>
@@ -436,7 +546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>20</v>
       </c>
@@ -444,7 +554,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>22</v>
       </c>
@@ -452,7 +562,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>24</v>
       </c>
@@ -460,13 +570,95 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AMJ23" s="1"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AMJ24" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -486,11 +678,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.8"/>
@@ -502,7 +694,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -510,7 +702,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -518,7 +710,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -526,7 +718,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,7 +726,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -542,23 +734,23 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -566,7 +758,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -574,7 +766,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -582,7 +774,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -590,24 +782,24 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="AMJ14" s="0"/>
     </row>
@@ -633,7 +825,7 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.12"/>
@@ -645,7 +837,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,7 +845,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -661,7 +853,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,7 +861,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,7 +869,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -685,7 +877,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -693,7 +885,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -701,7 +893,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -709,7 +901,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -717,7 +909,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -725,7 +917,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -733,24 +925,24 @@
         <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="AMJ14" s="0"/>
     </row>
@@ -776,7 +968,7 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.66"/>
   </cols>
@@ -786,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -794,7 +986,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,7 +1002,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,7 +1018,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -834,7 +1026,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -842,7 +1034,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,7 +1042,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,7 +1050,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,7 +1058,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -874,23 +1066,23 @@
         <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 9slice back button
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="106">
+  <si>
+    <t xml:space="preserve">generic.back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Back</t>
+  </si>
   <si>
     <t xml:space="preserve">menu.new_run</t>
   </si>
@@ -259,6 +265,9 @@
     <t xml:space="preserve">Her and her big sister rule the world. Be afraid Foddex, be afraid.</t>
   </si>
   <si>
+    <t xml:space="preserve">Tillbaka</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nytt spel</t>
   </si>
   <si>
@@ -301,6 +310,9 @@
     <t xml:space="preserve">Specialiteter</t>
   </si>
   <si>
+    <t xml:space="preserve">Πίσω</t>
+  </si>
+  <si>
     <t xml:space="preserve">Νέο παιχνίδι</t>
   </si>
   <si>
@@ -341,6 +353,9 @@
   </si>
   <si>
     <t xml:space="preserve">Ειδικότητες</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terug</t>
   </si>
   <si>
     <t xml:space="preserve">Nieuw Spel</t>
@@ -491,10 +506,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ30"/>
+  <dimension ref="A1:AMJ31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -519,10 +534,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -551,18 +566,18 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="0" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -679,13 +694,12 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="AMJ23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
@@ -703,6 +717,7 @@
       <c r="B25" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="AMJ25" s="1"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
@@ -742,6 +757,14 @@
       </c>
       <c r="B30" s="1" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -760,10 +783,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ14"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -778,23 +801,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -802,7 +826,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -810,7 +834,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -818,31 +842,31 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>66</v>
+      <c r="B7" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>67</v>
+      <c r="B8" s="0" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,7 +874,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,7 +882,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,26 +890,34 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="AMJ13" s="0"/>
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>42</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="AMJ14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="AMJ15" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -903,10 +935,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ14"/>
+  <dimension ref="A1:AMJ15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -918,26 +950,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>76</v>
+      <c r="B3" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -945,7 +978,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,7 +986,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -961,23 +994,23 @@
         <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>80</v>
+      <c r="B7" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>81</v>
+      <c r="B8" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,7 +1018,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,7 +1026,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1001,7 +1034,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,26 +1042,34 @@
         <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AMJ13" s="0"/>
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>87</v>
+      <c r="B14" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="AMJ14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AMJ15" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1046,10 +1087,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1062,7 +1103,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,15 +1111,15 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,7 +1127,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,7 +1135,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1102,23 +1143,23 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>94</v>
+      <c r="B8" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1126,7 +1167,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1134,7 +1175,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,7 +1183,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1150,15 +1191,15 @@
         <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,7 +1207,15 @@
         <v>42</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fake google translated all texts
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="197">
   <si>
     <t xml:space="preserve">generic.back</t>
   </si>
@@ -289,13 +289,13 @@
     <t xml:space="preserve">Tillbaka</t>
   </si>
   <si>
-    <t xml:space="preserve">Nytt spel</t>
+    <t xml:space="preserve">Ny körning</t>
   </si>
   <si>
     <t xml:space="preserve">Fortsätta</t>
   </si>
   <si>
-    <t xml:space="preserve">Inställningar</t>
+    <t xml:space="preserve">inställningar</t>
   </si>
   <si>
     <t xml:space="preserve">Databas</t>
@@ -307,6 +307,39 @@
     <t xml:space="preserve">Avsluta spelet</t>
   </si>
   <si>
+    <t xml:space="preserve">Mac "Maggot" the Hired Gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maggot använder lockbeten för att förvirra sina motståndare och kan tjäna pengar snabbare än någon annan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maggot är den häftigaste killen nummer ett på planeten. Han kan göra allt du inte kan. Ha. Han är riktigt cool. Försvinn nu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Den enda programmeraren som gjorde hela detta spel från grunden! Hurra!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foddex är den coolaste snubben i Neutropia. Han går in i en butik och matvarorna bara hoppar ner i hans korg. Det är rätt. Slå det nu!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michael "Souflaki" Stephanakis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Den enda speldesignern som gjorde hela detta spel från grunden! Parakalo!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr Souflaki är som Neutropiens själ. Utan honom skulle hela denna lilla shindig inte ens existera. Du gissade det. Gå bort!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofie ”Förstöraren” Oude Kotte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hon och hennes storasyster styr världen. Var rädd Foddex, var rädd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Något galet roligt.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Börja</t>
   </si>
   <si>
@@ -325,16 +358,49 @@
     <t xml:space="preserve">Jag är... Skötaren</t>
   </si>
   <si>
+    <t xml:space="preserve">Inga modifierare. En typisk tisdag.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vissa människor gillar utmaningar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Livet kommer att bli tufft.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Endast de starkaste kommer att överleva.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Karaktär</t>
   </si>
   <si>
-    <t xml:space="preserve">Specialiteter</t>
+    <t xml:space="preserve">Specialiseringar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karaktär Bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tecken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detta ger typ, du vet liksom, information om din karaktär och sånt. Välj en, jag bryr mig inte. Välj bara en och starta spelet. Hurra!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detta får dig att känna dig som en 6-årig tjej: extra speciell. Välj något fint, känn dig fancy. Du är speciell gurrrrl!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Svårigheter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lätt är lätt, svårt är svårt. Är det så svårt? Nej det var lätt. Bara spela spelet ordentligt.</t>
   </si>
   <si>
     <t xml:space="preserve">Πίσω</t>
   </si>
   <si>
-    <t xml:space="preserve">Νέο παιχνίδι</t>
+    <t xml:space="preserve">Νέα εκτέλεση</t>
   </si>
   <si>
     <t xml:space="preserve">Να συνεχίσει</t>
@@ -352,6 +418,39 @@
     <t xml:space="preserve">Κλείστε το παιχνίδι</t>
   </si>
   <si>
+    <t xml:space="preserve">Mac «Maggot» το Hired Gun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ο Μάγκοτ χρησιμοποιεί δόλωμα για να μπερδέψει τους αντιπάλους του και μπορεί να κερδίσει χρήματα πιο γρήγορα από οποιονδήποτε.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ο Μάγκοτ είναι ο νούμερο ένα φοβερός τύπος στον πλανήτη. Μπορεί να κάνει οτιδήποτε δεν μπορείτε. Χα. Είναι πραγματικά κουλ. Τώρα φύγε.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ο ένας και μοναδικός προγραμματιστής που έφτιαξε όλο αυτό το παιχνίδι από την αρχή! Ούρα!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ο Foddex είναι ο πιο κουλ μάγκας στο Neutropia. Μπαίνει σε ένα μαγαζί και τα παντοπωλεία απλώς πετάνε στο καλάθι του. Σωστά. Τώρα νικήστε το!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Μιχαήλ «Σουφλάκη» Στεφανάκης</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ο ένας και μοναδικός σχεδιαστής παιχνιδιών που έφτιαξε ολόκληρο αυτό το παιχνίδι από την αρχή! Παράκαλο!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ο κ. Σουφλάκη είναι σαν την ψυχή της Neutropia. Χωρίς αυτόν δεν θα υπήρχε καν όλος αυτός ο μικρός σκύλος. Το μάντεψες. Φύγε!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofie "The Destroyer" Oude Kotte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Αυτή και η μεγάλη της αδερφή κυβερνούν τον κόσμο. Να φοβάσαι Foddex, να φοβάσαι.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Κάτι τρελά αστείο.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Αρχίζουν</t>
   </si>
   <si>
@@ -364,22 +463,52 @@
     <t xml:space="preserve">Τζόκινγκ με τέρατα</t>
   </si>
   <si>
-    <t xml:space="preserve">Φοβάστε με βρωμερά θηρία!</t>
-  </si>
-  <si>
     <t xml:space="preserve">Είμαι… Ο οδοκαθαριστής</t>
   </si>
   <si>
+    <t xml:space="preserve">Χωρίς τροποποιητές. Μια τυπική Τρίτη.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Σε κάποιους αρέσουν οι προκλήσεις.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Η ζωή θα γίνει σκληρή.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Μόνο οι ισχυρότεροι θα επιβιώσουν.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Χαρακτήρας</t>
   </si>
   <si>
-    <t xml:space="preserve">Ειδικότητες</t>
+    <t xml:space="preserve">Εξειδικεύσεις</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Δέρμα</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Βιογραφικό χαρακτήρα</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Χαρακτήρες</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Αυτό δίνει όπως, ξέρετε, πληροφορίες για τον χαρακτήρα και τα πράγματα σας. Διάλεξε ένα, δεν με νοιάζει. Απλώς επιλέξτε ένα και ξεκινήστε το παιχνίδι. Ούρα!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Αυτό σας κάνει να νιώθετε σαν ένα 6χρονο κορίτσι: πολύ ιδιαίτερο. Διαλέξτε κάτι φανταχτερό, νιώστε φανταχτερό. Είσαι speciul gurrrrl!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Δυσκολίες</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Το εύκολο είναι εύκολο, το δύσκολο είναι δύσκολο. Είναι τόσο δύσκολο; Όχι, ήταν εύκολο. Απλώς παίξτε το παιχνίδι.</t>
   </si>
   <si>
     <t xml:space="preserve">Terug</t>
   </si>
   <si>
-    <t xml:space="preserve">Nieuw Spel</t>
+    <t xml:space="preserve">Nieuwe loop</t>
   </si>
   <si>
     <t xml:space="preserve">Doorgaan</t>
@@ -391,10 +520,46 @@
     <t xml:space="preserve">Databank</t>
   </si>
   <si>
-    <t xml:space="preserve">Spel Afsluiten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start</t>
+    <t xml:space="preserve">Sluit het spel af</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mac "Mad" de ingehuurde kanon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maggot gebruikt lokvogels om zijn tegenstanders in de war te brengen en kan sneller dan wie dan ook geld verdienen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maggot is de nummer één geweldigste kerel ter wereld. Hij kan alles wat jij niet kunt. Ha. Hij is echt cool. Ga nu weg.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marc "Foddex" Oude Kotte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De enige echte programmeur die dit hele spel helemaal opnieuw heeft gemaakt! Hoera!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Foddex is de coolste kerel in Neutropia. Hij gaat een winkel binnen en de boodschappen springen gewoon in zijn mandje. Dat is juist. Versla het nu!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michaël "Souflaki" Stephanakis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">De enige echte game-ontwerper die deze hele game vanaf nul heeft gemaakt! Parakalo!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meneer Souflaki is als de ziel van Neutropia. Zonder hem zou deze hele kleine shindig niet eens bestaan. Je hebt het geraden. Ga weg!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofie "De Vernietiger" Oude Kotte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zij en haar grote zus regeren de wereld. Wees bang Foddex, wees bang.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iets waanzinnig grappigs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beginnen</t>
   </si>
   <si>
     <t xml:space="preserve">Moeilijkheidsgraad</t>
@@ -409,13 +574,46 @@
     <t xml:space="preserve">Vrees me vuile beesten!</t>
   </si>
   <si>
-    <t xml:space="preserve">Ik ben... de Allesvreter</t>
+    <t xml:space="preserve">Ik ben... de aaseter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Geen modificaties. Een typische dinsdag.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sommige mensen houden van uitdagingen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Het leven zal zwaar worden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alleen de sterkste zal overleven.</t>
   </si>
   <si>
     <t xml:space="preserve">Karakter</t>
   </si>
   <si>
-    <t xml:space="preserve">Specialiteiten</t>
+    <t xml:space="preserve">Specialisaties</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karakter bio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karakters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dit geeft zoals, je weet wel, informatie over je personage en zo. Kies er een, het kan me niet schelen. Selecteer er gewoon een en start het spel. Hoera!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hierdoor voel je je net een meisje van 6: extra bijzonder. Kies iets speciaals, voel je chique. Je bent speciul gurrrrl!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moeilijkheden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Makkelijk is makkelijk, moeilijk is moeilijk. Is dat zo moeilijk? Nee dat was makkelijk toch. Speel het spel nou maar.</t>
   </si>
 </sst>
 </file>
@@ -523,11 +721,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30:B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.33984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.7"/>
   </cols>
@@ -903,15 +1101,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ15"/>
+  <dimension ref="A1:AMJ44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30:B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.8"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="10.5"/>
   </cols>
@@ -975,7 +1173,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>94</v>
@@ -983,61 +1181,293 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>42</v>
+      <c r="A10" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="AMJ14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="AMJ15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="B23" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="B24" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="B25" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="AMJ14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="B34" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="AMJ15" s="0"/>
+      <c r="B35" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1055,15 +1485,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ15"/>
+  <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30:B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.12"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="10.5"/>
   </cols>
@@ -1073,16 +1503,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1090,7 +1520,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1098,7 +1528,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1106,7 +1536,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1114,7 +1544,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1122,74 +1552,306 @@
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="AMJ14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AMJ15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B20" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="B21" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="B22" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="B23" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="B25" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="AMJ14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="B34" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AMJ15" s="0"/>
+      <c r="B35" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>159</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1207,15 +1869,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B43" activeCellId="1" sqref="B30:B33 B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,7 +1885,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1231,7 +1893,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1239,7 +1901,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>119</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1247,7 +1909,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>120</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1255,7 +1917,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,71 +1933,303 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>122</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B20" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="B21" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="B22" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="B23" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="B24" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="B25" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="B34" s="0" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="0" t="s">
-        <v>130</v>
+      <c r="B35" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extra long bio text
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">character1.bio</t>
   </si>
   <si>
-    <t xml:space="preserve">Maggot is the number one awesomest dude on the planet. He can do anything you can’t. Ha. He’s really cool. Now go away.</t>
+    <t xml:space="preserve">Maggot is the number one awesomest dude on the planet. He can do anything you can’t. Ha. He’s really cool. He’s the man. He’s the shit. He’s the bro. He’s dudest dude of anyone who ever duded.</t>
   </si>
   <si>
     <t xml:space="preserve">character2.name</t>
@@ -283,7 +283,7 @@
     <t xml:space="preserve">newrun.popup.difficulty.text</t>
   </si>
   <si>
-    <t xml:space="preserve">Easy is easy, hard is hard. Is that so hard? No that was easy right. Just play the game aight.</t>
+    <t xml:space="preserve">Easy is easy, hard is hard. Is that so hard? No that was easy right. Just play the game aight. Extra long text that will run out of the screen hopefully. Just keep on writing text Marc. Write it! Write it for glory!</t>
   </si>
   <si>
     <t xml:space="preserve">Tillbaka</t>
@@ -721,11 +721,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30:B33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.3125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.7"/>
   </cols>
@@ -1104,14 +1104,14 @@
   <dimension ref="A1:AMJ44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30:B33"/>
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,15 +1487,15 @@
   </sheetPr>
   <dimension ref="A1:AMJ44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30:B33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.12"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1872,10 +1872,10 @@
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B43" activeCellId="1" sqref="B30:B33 B43"/>
+      <selection pane="topLeft" activeCell="B43" activeCellId="0" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.41015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.7"/>
   </cols>

</xml_diff>

<commit_message>
Added bio's to hero configuration
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -73,19 +73,55 @@
     <t xml:space="preserve">CHARACTER</t>
   </si>
   <si>
-    <t xml:space="preserve">character1.name</t>
+    <t xml:space="preserve">maggot.name</t>
   </si>
   <si>
     <t xml:space="preserve">Mac “Maggot” the Hired Gun</t>
   </si>
   <si>
-    <t xml:space="preserve">character1.description</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">maggot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.description</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Maggot uses decoys to confuse his opponents and can earn money faster than anyone.</t>
   </si>
   <si>
-    <t xml:space="preserve">character1.bio</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">maggot</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.bio</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Maggot is the number one awesomest dude on the planet. He can do anything you can’t. Ha. He’s really cool. He’s the man. He’s the shit. He’s the bro. He’s dudest dude of anyone who ever duded.</t>
@@ -632,7 +668,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -662,6 +698,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -706,7 +748,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -716,6 +758,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -742,11 +788,11 @@
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
@@ -824,7 +870,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -833,7 +879,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1133,11 +1179,11 @@
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
@@ -1216,7 +1262,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1225,7 +1271,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1525,11 +1571,11 @@
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.40234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
@@ -1608,7 +1654,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1617,7 +1663,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1652,7 +1698,7 @@
       <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="4" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1917,11 +1963,11 @@
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A:A"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.36328125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.35546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
@@ -1999,7 +2045,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
@@ -2008,7 +2054,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="0" t="s">

</xml_diff>

<commit_message>
Last changes to configuration
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">CHARACTER</t>
   </si>
   <si>
-    <t xml:space="preserve">maggot.name</t>
+    <t xml:space="preserve">characters.maggot.name</t>
   </si>
   <si>
     <t xml:space="preserve">Mac “Maggot” the Hired Gun</t>
@@ -86,7 +86,79 @@
         <rFont val="Calibri"/>
         <family val="0"/>
       </rPr>
-      <t xml:space="preserve">maggot</t>
+      <t xml:space="preserve">characters.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">maggot.description</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Maggot uses decoys to confuse his opponents and can earn money faster than anyone.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">characters.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">maggot.bio</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Maggot is the number one awesomest dude on the planet. He can do anything you can’t. Ha. He’s really cool. He’s the man. He’s the shit. He’s the bro. He’s dudest dude of anyone who ever duded.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">characters.hero</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2.name</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Marc “Foddex” Oude Kotte</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">characters.hero2</t>
     </r>
     <r>
       <rPr>
@@ -100,7 +172,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Maggot uses decoys to confuse his opponents and can earn money faster than anyone.</t>
+    <t xml:space="preserve">The one and only programmer that made this entire game from scratch! Hurray!</t>
   </si>
   <si>
     <r>
@@ -110,7 +182,7 @@
         <rFont val="Calibri"/>
         <family val="0"/>
       </rPr>
-      <t xml:space="preserve">maggot</t>
+      <t xml:space="preserve">characters.hero2</t>
     </r>
     <r>
       <rPr>
@@ -124,58 +196,148 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Maggot is the number one awesomest dude on the planet. He can do anything you can’t. Ha. He’s really cool. He’s the man. He’s the shit. He’s the bro. He’s dudest dude of anyone who ever duded.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character2.name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marc “Foddex” Oude Kotte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character2.description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The one and only programmer that made this entire game from scratch! Hurray!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">character2.bio</t>
-  </si>
-  <si>
     <t xml:space="preserve">Foddex is the coolest dude in Neutropia. He goes into a store and the groceries just jump into his basket. That’s right. Now beat it!</t>
   </si>
   <si>
-    <t xml:space="preserve">character3.name</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">characters.hero3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.name</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Michael “Souvlaki” Stephanakis</t>
   </si>
   <si>
-    <t xml:space="preserve">character3.description</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">characters.hero3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">description</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">The one and only game designer that made this entire game from scratch! Parakalo!</t>
   </si>
   <si>
-    <t xml:space="preserve">character3.bio</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">characters.hero3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.bio</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Mr. Souvlaki is like the soul of Neutropia. Without him this whole little shindig wouldn’t even exist. You guessed it. Go away!</t>
   </si>
   <si>
-    <t xml:space="preserve">character4.name</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">characters.hero4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.name</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Sofie “The Destroyer” Oude Kotte</t>
   </si>
   <si>
-    <t xml:space="preserve">character4.description</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">characters.hero4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.description</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Her and her big sister rule the world. Be afraid Foddex, be afraid.</t>
   </si>
   <si>
-    <t xml:space="preserve">character4.bio</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">characters.hero4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.bio</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Something insanely funny.</t>
@@ -766,7 +928,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -788,11 +950,11 @@
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B8:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.28125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.2734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
@@ -887,7 +1049,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -895,7 +1057,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -903,7 +1065,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -911,7 +1073,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -919,7 +1081,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -927,7 +1089,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -935,7 +1097,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -943,7 +1105,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -951,7 +1113,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="0" t="s">
@@ -1180,10 +1342,10 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
@@ -1279,7 +1441,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1287,7 +1449,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1295,7 +1457,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1303,7 +1465,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1311,7 +1473,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1319,7 +1481,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1327,7 +1489,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1335,7 +1497,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1343,7 +1505,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1572,10 +1734,10 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.39453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
@@ -1671,7 +1833,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1679,7 +1841,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1687,15 +1849,15 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1703,7 +1865,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1711,7 +1873,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1719,7 +1881,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1727,7 +1889,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1735,7 +1897,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1963,11 +2125,11 @@
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.35546875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
@@ -2062,7 +2224,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C11" s="0" t="s">
@@ -2070,7 +2232,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C12" s="0" t="s">
@@ -2078,7 +2240,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="0" t="s">
@@ -2086,7 +2248,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="0" t="s">
@@ -2094,7 +2256,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="0" t="s">
@@ -2102,7 +2264,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="0" t="s">
@@ -2110,7 +2272,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="0" t="s">
@@ -2118,7 +2280,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="0" t="s">
@@ -2126,7 +2288,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="0" t="s">

</xml_diff>

<commit_message>
First work on legend
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="203">
   <si>
     <t xml:space="preserve">MAIN MENU</t>
   </si>
@@ -79,265 +79,67 @@
     <t xml:space="preserve">Mac “Maggot” the Hired Gun</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">characters.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">maggot.description</t>
-    </r>
+    <t xml:space="preserve">characters.maggot.description</t>
   </si>
   <si>
     <t xml:space="preserve">Maggot uses decoys to confuse his opponents and can earn money faster than anyone.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">characters.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">maggot.bio</t>
-    </r>
+    <t xml:space="preserve">characters.maggot.bio</t>
   </si>
   <si>
     <t xml:space="preserve">Maggot is the number one awesomest dude on the planet. He can do anything you can’t. Ha. He’s really cool. He’s the man. He’s the shit. He’s the bro. He’s dudest dude of anyone who ever duded.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">characters.hero</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">2.name</t>
-    </r>
+    <t xml:space="preserve">characters.hero2.name</t>
   </si>
   <si>
     <t xml:space="preserve">Marc “Foddex” Oude Kotte</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">characters.hero2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.description</t>
-    </r>
+    <t xml:space="preserve">characters.hero2.description</t>
   </si>
   <si>
     <t xml:space="preserve">The one and only programmer that made this entire game from scratch! Hurray!</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">characters.hero2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.bio</t>
-    </r>
+    <t xml:space="preserve">characters.hero2.bio</t>
   </si>
   <si>
     <t xml:space="preserve">Foddex is the coolest dude in Neutropia. He goes into a store and the groceries just jump into his basket. That’s right. Now beat it!</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">characters.hero3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.name</t>
-    </r>
+    <t xml:space="preserve">characters.hero3.name</t>
   </si>
   <si>
     <t xml:space="preserve">Michael “Souvlaki” Stephanakis</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">characters.hero3.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">description</t>
-    </r>
+    <t xml:space="preserve">characters.hero3.description</t>
   </si>
   <si>
     <t xml:space="preserve">The one and only game designer that made this entire game from scratch! Parakalo!</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">characters.hero3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.bio</t>
-    </r>
+    <t xml:space="preserve">characters.hero3.bio</t>
   </si>
   <si>
     <t xml:space="preserve">Mr. Souvlaki is like the soul of Neutropia. Without him this whole little shindig wouldn’t even exist. You guessed it. Go away!</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">characters.hero4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.name</t>
-    </r>
+    <t xml:space="preserve">characters.hero4.name</t>
   </si>
   <si>
     <t xml:space="preserve">Sofie “The Destroyer” Oude Kotte</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">characters.hero4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.description</t>
-    </r>
+    <t xml:space="preserve">characters.hero4.description</t>
   </si>
   <si>
     <t xml:space="preserve">Her and her big sister rule the world. Be afraid Foddex, be afraid.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">characters.hero4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.bio</t>
-    </r>
+    <t xml:space="preserve">characters.hero4.bio</t>
   </si>
   <si>
     <t xml:space="preserve">Something insanely funny.</t>
@@ -491,6 +293,15 @@
   </si>
   <si>
     <t xml:space="preserve">Easy is easy, hard is hard. Is that so hard? No that was easy right. Just play the game aight. Extra long text that will run out of the screen hopefully. Just keep on writing text Marc. Write it! Write it for glory!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map.legend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legend</t>
   </si>
   <si>
     <t xml:space="preserve">Tillbaka</t>
@@ -830,7 +641,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -860,12 +671,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -910,24 +715,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -944,107 +745,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B8:B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="45:45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1052,7 +853,7 @@
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1060,7 +861,7 @@
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1068,7 +869,7 @@
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1076,7 +877,7 @@
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1084,7 +885,7 @@
       <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1092,7 +893,7 @@
       <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1100,7 +901,7 @@
       <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1108,7 +909,7 @@
       <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1116,211 +917,222 @@
       <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1335,116 +1147,116 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8:B10"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="45:45 B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="11.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="11.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>90</v>
+      <c r="C1" s="3" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>91</v>
+      <c r="C2" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>92</v>
+      <c r="C3" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>93</v>
+      <c r="C4" s="3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>94</v>
+      <c r="C5" s="3" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>95</v>
+      <c r="C6" s="3" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>96</v>
+      <c r="C7" s="3" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>97</v>
+      <c r="C8" s="3" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>98</v>
+      <c r="C9" s="3" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>99</v>
+      <c r="C10" s="3" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1452,272 +1264,272 @@
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>100</v>
+      <c r="C12" s="3" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>101</v>
+      <c r="C13" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>102</v>
+      <c r="C14" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>103</v>
+      <c r="C15" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>104</v>
+      <c r="C16" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>105</v>
+      <c r="C17" s="3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>106</v>
+      <c r="C18" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>107</v>
+      <c r="C19" s="3" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>108</v>
+      <c r="C20" s="3" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>109</v>
+      <c r="C21" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>110</v>
+      <c r="C22" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>111</v>
+      <c r="C23" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>112</v>
+      <c r="C24" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>113</v>
+      <c r="C25" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>114</v>
+      <c r="C26" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>115</v>
+      <c r="C27" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>116</v>
+      <c r="C28" s="3" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>117</v>
+      <c r="C29" s="3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>118</v>
+      <c r="C34" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>119</v>
+      <c r="C35" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>120</v>
+      <c r="C36" s="3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>121</v>
+      <c r="C38" s="3" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>124</v>
+      <c r="C42" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>125</v>
+      <c r="C43" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>126</v>
+      <c r="C44" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -1727,116 +1539,116 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8:B10"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="45:45 B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="16.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>127</v>
+      <c r="C1" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>128</v>
+      <c r="C2" s="3" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>129</v>
+      <c r="C3" s="3" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>130</v>
+      <c r="C4" s="3" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>131</v>
+      <c r="C5" s="3" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>132</v>
+      <c r="C6" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>133</v>
+      <c r="C7" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>134</v>
+      <c r="C8" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>135</v>
+      <c r="C9" s="3" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>136</v>
+      <c r="C10" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1844,272 +1656,272 @@
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>137</v>
+      <c r="C12" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>138</v>
+      <c r="C13" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>139</v>
+      <c r="C14" s="3" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>140</v>
+      <c r="C15" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>141</v>
+      <c r="C16" s="3" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>142</v>
+      <c r="C17" s="3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>143</v>
+      <c r="C18" s="3" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>144</v>
+      <c r="C19" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>145</v>
+      <c r="C20" s="3" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>146</v>
+      <c r="C21" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>147</v>
+      <c r="C22" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>148</v>
+      <c r="C23" s="3" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>149</v>
+      <c r="C25" s="3" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>150</v>
+      <c r="C26" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>151</v>
+      <c r="C27" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>152</v>
+      <c r="C28" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>153</v>
+      <c r="C29" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>154</v>
+      <c r="C34" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>155</v>
+      <c r="C35" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>156</v>
+      <c r="C36" s="3" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>157</v>
+      <c r="C38" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>160</v>
+      <c r="C42" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>161</v>
+      <c r="C43" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>162</v>
+      <c r="C44" s="3" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
@@ -2119,384 +1931,388 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8:B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="45:45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>163</v>
+      <c r="C1" s="3" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>164</v>
+      <c r="C2" s="3" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>165</v>
+      <c r="C3" s="3" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>166</v>
+      <c r="C4" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>167</v>
+      <c r="C5" s="3" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>168</v>
+      <c r="C7" s="3" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>169</v>
+      <c r="C8" s="3" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>170</v>
+      <c r="C9" s="1" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>171</v>
+      <c r="C10" s="1" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>172</v>
+      <c r="C11" s="1" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>173</v>
+      <c r="C12" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>174</v>
+      <c r="C13" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>175</v>
+      <c r="C14" s="1" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>176</v>
+      <c r="C15" s="1" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>177</v>
+      <c r="C16" s="1" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>178</v>
+      <c r="C17" s="1" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>179</v>
+      <c r="C18" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>180</v>
+      <c r="C19" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>181</v>
+      <c r="C20" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>182</v>
+      <c r="C21" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>183</v>
+      <c r="C22" s="1" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>184</v>
+      <c r="C23" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>185</v>
+      <c r="C24" s="1" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>186</v>
+      <c r="C25" s="1" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>187</v>
+      <c r="C26" s="1" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="0" t="s">
-        <v>188</v>
+      <c r="C27" s="1" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C28" s="0" t="s">
-        <v>189</v>
+      <c r="C28" s="1" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>190</v>
+      <c r="C29" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="0" t="s">
-        <v>191</v>
+      <c r="C34" s="1" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C35" s="0" t="s">
-        <v>192</v>
+      <c r="C35" s="1" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C36" s="0" t="s">
-        <v>193</v>
+      <c r="C36" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C38" s="0" t="s">
-        <v>194</v>
+      <c r="C38" s="1" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>192</v>
-      </c>
-    </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="0" t="s">
-        <v>197</v>
+      <c r="C42" s="1" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C43" s="0" t="s">
-        <v>198</v>
+      <c r="C43" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="0" t="s">
-        <v>199</v>
-      </c>
+      <c r="C44" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0"/>
+      <c r="B45" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Worked on hud + cards
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="223">
   <si>
     <t xml:space="preserve">MAIN MENU</t>
   </si>
@@ -302,6 +302,66 @@
   </si>
   <si>
     <t xml:space="preserve">Legend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card.type.attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card.type.gambit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gambit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card.type.gear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARD TEST (TEMP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card.name.test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Auto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card.text.test1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Only Foddex ever goes Full Auto, until now!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card.name.test2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card.text.test2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofie is the destroyer. Fear her.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card.name.test3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card.text.test3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Never anger the wife. Life is better that way.</t>
   </si>
   <si>
     <t xml:space="preserve">Tillbaka</t>
@@ -749,10 +809,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="45:45"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1133,6 +1193,84 @@
       </c>
       <c r="C45" s="1" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1154,7 +1292,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="45:45 B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1172,7 +1310,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1180,7 +1318,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,7 +1326,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1196,7 +1334,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1204,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1212,7 +1350,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1220,7 +1358,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1231,7 +1369,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1240,7 +1378,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1249,7 +1387,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1265,7 +1403,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1273,7 +1411,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1281,7 +1419,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1289,7 +1427,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1297,7 +1435,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,7 +1443,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>108</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1313,7 +1451,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>109</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1321,7 +1459,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>110</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1332,7 +1470,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>111</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1340,7 +1478,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1348,7 +1486,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>113</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1356,7 +1494,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>114</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1364,7 +1502,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1372,7 +1510,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,7 +1518,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1388,7 +1526,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1396,7 +1534,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1404,7 +1542,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1444,7 +1582,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1452,7 +1590,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1460,7 +1598,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,7 +1614,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,7 +1622,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1492,7 +1630,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,7 +1638,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,7 +1646,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,7 +1654,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,7 +1662,7 @@
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1546,7 +1684,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="45:45 B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1564,7 +1702,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1572,7 +1710,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1580,7 +1718,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1588,7 +1726,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1596,7 +1734,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,7 +1742,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,7 +1750,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,7 +1761,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,7 +1770,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1641,7 +1779,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1657,7 +1795,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1665,7 +1803,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1673,7 +1811,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1681,7 +1819,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,7 +1827,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1697,7 +1835,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1705,7 +1843,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1713,7 +1851,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1724,7 +1862,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,7 +1870,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,7 +1878,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,7 +1886,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,7 +1902,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,7 +1910,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,7 +1918,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,7 +1926,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1796,7 +1934,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1836,7 +1974,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1844,7 +1982,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1852,7 +1990,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1868,7 +2006,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1876,7 +2014,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1884,7 +2022,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1892,7 +2030,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1900,7 +2038,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1908,7 +2046,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>164</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1916,7 +2054,7 @@
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>165</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1935,10 +2073,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="45:45"/>
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1955,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>166</v>
+        <v>186</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1963,7 +2101,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>167</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1971,7 +2109,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>168</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1979,7 +2117,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>169</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1987,7 +2125,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2003,7 +2141,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,7 +2152,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,7 +2161,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,7 +2170,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>174</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2040,7 +2178,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>175</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2048,7 +2186,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,7 +2194,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2064,7 +2202,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>178</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2072,7 +2210,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,7 +2218,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>180</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,7 +2226,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2096,7 +2234,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,7 +2242,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,7 +2253,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2123,7 +2261,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>185</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2131,7 +2269,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>186</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2139,7 +2277,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>187</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2147,7 +2285,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>188</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2155,7 +2293,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>189</v>
+        <v>209</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2163,7 +2301,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2171,7 +2309,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>191</v>
+        <v>211</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2179,7 +2317,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>192</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2187,7 +2325,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2227,7 +2365,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>194</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2235,7 +2373,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,7 +2381,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>196</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2259,7 +2397,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>197</v>
+        <v>217</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2267,7 +2405,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>198</v>
+        <v>218</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2275,7 +2413,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2283,7 +2421,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>195</v>
+        <v>215</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2291,7 +2429,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2299,7 +2437,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>201</v>
+        <v>221</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2307,12 +2445,8 @@
         <v>88</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0"/>
-      <c r="B45" s="0"/>
+        <v>222</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Added more test cards
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="227">
   <si>
     <t xml:space="preserve">MAIN MENU</t>
   </si>
@@ -337,7 +337,7 @@
     <t xml:space="preserve">card.text.test1</t>
   </si>
   <si>
-    <t xml:space="preserve">Only Foddex ever goes Full Auto, until now!</t>
+    <t xml:space="preserve">Only Foddex ever went Full Auto, until now!</t>
   </si>
   <si>
     <t xml:space="preserve">card.name.test2</t>
@@ -362,6 +362,18 @@
   </si>
   <si>
     <t xml:space="preserve">Never anger the wife. Life is better that way.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card.name.test4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Michalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">card.text.test4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fear the Artist!</t>
   </si>
   <si>
     <t xml:space="preserve">Tillbaka</t>
@@ -809,10 +821,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
+      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.2734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1229,7 +1241,7 @@
       <c r="B49" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1237,7 +1249,7 @@
       <c r="B50" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1245,7 +1257,7 @@
       <c r="B51" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1253,7 +1265,7 @@
       <c r="B52" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1261,7 +1273,7 @@
       <c r="B53" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1269,8 +1281,24 @@
       <c r="B54" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="1" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B56" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1310,7 +1338,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1318,7 +1346,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1326,7 +1354,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1334,7 +1362,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1342,7 +1370,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1350,7 +1378,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1358,7 +1386,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1369,7 +1397,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1378,7 +1406,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1387,7 +1415,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1403,7 +1431,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1411,7 +1439,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1419,7 +1447,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,7 +1455,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,7 +1463,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,7 +1471,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1451,7 +1479,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1459,7 +1487,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1470,7 +1498,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1478,7 +1506,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1486,7 +1514,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1494,7 +1522,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1502,7 +1530,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,7 +1538,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1518,7 +1546,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1526,7 +1554,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1534,7 +1562,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1542,7 +1570,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1582,7 +1610,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1590,7 +1618,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1598,7 +1626,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1614,7 +1642,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,7 +1650,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,7 +1658,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,7 +1666,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,7 +1674,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1654,7 +1682,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,7 +1690,7 @@
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -1702,7 +1730,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,7 +1738,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1718,7 +1746,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,7 +1754,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,7 +1762,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,7 +1770,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1750,7 +1778,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1761,7 +1789,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1770,7 +1798,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1779,7 +1807,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1795,7 +1823,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1803,7 +1831,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,7 +1839,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1819,7 +1847,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1827,7 +1855,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1835,7 +1863,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1843,7 +1871,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,7 +1879,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1862,7 +1890,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1870,7 +1898,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1878,7 +1906,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,7 +1914,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1902,7 +1930,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1910,7 +1938,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1918,7 +1946,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1926,7 +1954,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1934,7 +1962,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1974,7 +2002,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1982,7 +2010,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1990,7 +2018,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2006,7 +2034,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2014,7 +2042,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2022,7 +2050,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2030,7 +2058,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2038,7 +2066,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2046,7 +2074,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2054,7 +2082,7 @@
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2093,7 +2121,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2101,7 +2129,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2109,7 +2137,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2117,7 +2145,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2125,7 +2153,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2141,7 +2169,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2180,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2161,7 +2189,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2170,7 +2198,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,7 +2206,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2186,7 +2214,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2194,7 +2222,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2202,7 +2230,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2210,7 +2238,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2218,7 +2246,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2226,7 +2254,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2234,7 +2262,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2242,7 +2270,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2253,7 +2281,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2261,7 +2289,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2269,7 +2297,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2277,7 +2305,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2285,7 +2313,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2293,7 +2321,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2301,7 +2329,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2309,7 +2337,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2317,7 +2345,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2325,7 +2353,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2365,7 +2393,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2373,7 +2401,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2381,7 +2409,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2397,7 +2425,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2405,7 +2433,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2413,7 +2441,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2421,7 +2449,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2429,7 +2457,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2437,7 +2465,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2445,7 +2473,7 @@
         <v>88</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added end turn 9sliced
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="233">
   <si>
     <t xml:space="preserve">MAIN MENU</t>
   </si>
@@ -376,6 +376,15 @@
     <t xml:space="preserve">Fear the Artist!</t>
   </si>
   <si>
+    <t xml:space="preserve">GAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">game.endturn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End Turn</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tillbaka</t>
   </si>
   <si>
@@ -487,6 +496,9 @@
     <t xml:space="preserve">Lätt är lätt, svårt är svårt. Är det så svårt? Nej det var lätt. Bara spela spelet ordentligt.</t>
   </si>
   <si>
+    <t xml:space="preserve">Avsluta Tur</t>
+  </si>
+  <si>
     <t xml:space="preserve">Πίσω</t>
   </si>
   <si>
@@ -595,6 +607,9 @@
     <t xml:space="preserve">Το εύκολο είναι εύκολο, το δύσκολο είναι δύσκολο. Είναι τόσο δύσκολο; Όχι, ήταν εύκολο. Απλώς παίξτε το παιχνίδι.</t>
   </si>
   <si>
+    <t xml:space="preserve">Τέλος στροφής</t>
+  </si>
+  <si>
     <t xml:space="preserve">Terug</t>
   </si>
   <si>
@@ -704,6 +719,9 @@
   </si>
   <si>
     <t xml:space="preserve">Makkelijk is makkelijk, moeilijk is moeilijk. Is dat zo moeilijk? Nee dat was makkelijk toch. Speel het spel nou maar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einde Beurt</t>
   </si>
 </sst>
 </file>
@@ -817,17 +835,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C51" activeCellId="0" sqref="C51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.2734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.7"/>
@@ -1299,6 +1317,17 @@
       </c>
       <c r="C56" s="1" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1313,17 +1342,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.7"/>
@@ -1338,7 +1367,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,7 +1375,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1354,7 +1383,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1362,7 +1391,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1370,7 +1399,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1378,7 +1407,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1386,7 +1415,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1397,7 +1426,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,7 +1435,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1415,7 +1444,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1431,7 +1460,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1439,7 +1468,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1447,7 +1476,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1455,7 +1484,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1463,7 +1492,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1471,7 +1500,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1479,7 +1508,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1487,7 +1516,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1498,7 +1527,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1506,7 +1535,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1514,7 +1543,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1522,7 +1551,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,7 +1559,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1538,7 +1567,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1546,7 +1575,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1554,7 +1583,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1562,7 +1591,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1570,7 +1599,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,7 +1639,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1618,7 +1647,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1626,7 +1655,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1642,7 +1671,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,7 +1679,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1658,7 +1687,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1666,7 +1695,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1674,7 +1703,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1682,7 +1711,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,7 +1719,18 @@
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>153</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -1705,17 +1745,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C45" activeCellId="0" sqref="C45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.38671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.7"/>
@@ -1730,7 +1770,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1738,7 +1778,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1746,7 +1786,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1754,7 +1794,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1762,7 +1802,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1770,7 +1810,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1778,7 +1818,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1789,7 +1829,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1798,7 +1838,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1807,7 +1847,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,7 +1863,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1831,7 +1871,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1839,7 +1879,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,7 +1887,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1855,7 +1895,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,7 +1903,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1871,7 +1911,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1879,7 +1919,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1890,7 +1930,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1898,7 +1938,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1906,7 +1946,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1914,7 +1954,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,7 +1970,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,7 +1978,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,7 +1986,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1954,7 +1994,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1962,7 +2002,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2002,7 +2042,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2010,7 +2050,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2018,7 +2058,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2034,7 +2074,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,7 +2082,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,7 +2090,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2058,7 +2098,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,7 +2106,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2074,7 +2114,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2082,7 +2122,18 @@
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>189</v>
+        <v>193</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2097,17 +2148,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.34765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.33984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.7"/>
@@ -2121,7 +2172,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2129,7 +2180,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2137,7 +2188,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2145,7 +2196,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2153,7 +2204,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2169,7 +2220,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,7 +2231,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>196</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2189,7 +2240,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2198,7 +2249,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2206,7 +2257,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2214,7 +2265,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2222,7 +2273,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2230,7 +2281,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2238,7 +2289,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2246,7 +2297,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,7 +2305,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2262,7 +2313,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2270,7 +2321,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>207</v>
+        <v>212</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,7 +2332,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2289,7 +2340,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,7 +2348,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>210</v>
+        <v>215</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,7 +2356,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2313,7 +2364,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2321,7 +2372,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2329,7 +2380,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2337,7 +2388,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,7 +2396,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2353,7 +2404,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2393,7 +2444,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2401,7 +2452,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2409,7 +2460,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2425,7 +2476,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2433,7 +2484,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2441,7 +2492,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2449,7 +2500,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,7 +2508,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2465,7 +2516,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2473,7 +2524,18 @@
         <v>88</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>226</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on selecting specializations
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="243">
   <si>
     <t xml:space="preserve">MAIN MENU</t>
   </si>
@@ -293,6 +293,36 @@
   </si>
   <si>
     <t xml:space="preserve">Easy is easy, hard is hard. Is that so hard? No that was easy right. Just play the game aight. Extra long text that will run out of the screen hopefully. Just keep on writing text Marc. Write it! Write it for glory!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newrun.specializations.group.armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Armor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newrun.specializations.group.melee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newrun.specializations.group.subsonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newrun.specializations.group.firearms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firearms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newrun.specializations.group.scitech</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sci-Tech</t>
   </si>
   <si>
     <t xml:space="preserve">MAP</t>
@@ -835,14 +865,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A57" activeCellId="0" sqref="A57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1215,87 +1245,87 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="2" t="s">
+      <c r="B45" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C45" s="1" t="s">
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="1" t="s">
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="1" t="s">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B48" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C48" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="1" t="s">
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="2" t="s">
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B50" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="1" t="s">
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C53" s="1" t="s">
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="1" t="s">
         <v>111</v>
       </c>
@@ -1320,14 +1350,54 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C57" s="0" t="s">
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="1" t="s">
         <v>119</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1342,14 +1412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1367,7 +1437,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1375,7 +1445,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1383,7 +1453,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1391,7 +1461,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1399,7 +1469,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,7 +1477,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1415,7 +1485,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1426,7 +1496,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1435,7 +1505,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1444,7 +1514,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1460,7 +1530,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,7 +1538,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,7 +1546,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,7 +1554,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1492,7 +1562,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>134</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,7 +1570,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,7 +1578,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1516,7 +1586,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1527,7 +1597,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,7 +1605,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>139</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1543,7 +1613,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1551,7 +1621,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1559,7 +1629,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1567,7 +1637,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1575,7 +1645,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1583,7 +1653,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1591,7 +1661,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1599,7 +1669,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1639,7 +1709,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1647,7 +1717,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1655,7 +1725,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,7 +1741,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1679,7 +1749,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1687,7 +1757,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1695,7 +1765,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1703,7 +1773,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,7 +1781,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,20 +1789,21 @@
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
+        <v>128</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -1745,7 +1816,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1770,7 +1841,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1778,7 +1849,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1786,7 +1857,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1794,7 +1865,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1802,7 +1873,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1810,7 +1881,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1818,7 +1889,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1829,7 +1900,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1838,7 +1909,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1847,7 +1918,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1863,7 +1934,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1871,7 +1942,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1879,7 +1950,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1887,7 +1958,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1895,7 +1966,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,7 +1974,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1911,7 +1982,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1919,7 +1990,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1930,7 +2001,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1938,7 +2009,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,7 +2017,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1954,7 +2025,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>179</v>
+        <v>189</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1970,7 +2041,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1978,7 +2049,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>181</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1986,7 +2057,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>182</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1994,7 +2065,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2002,7 +2073,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2042,7 +2113,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>185</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2050,7 +2121,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2058,7 +2129,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>187</v>
+        <v>197</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2074,7 +2145,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2082,7 +2153,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2090,7 +2161,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2098,7 +2169,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2106,7 +2177,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2114,7 +2185,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>192</v>
+        <v>202</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2122,18 +2193,18 @@
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>193</v>
+        <v>203</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>194</v>
+        <v>128</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -2148,7 +2219,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2172,7 +2243,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>195</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,7 +2251,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2188,7 +2259,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2267,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2204,7 +2275,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2220,7 +2291,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2231,7 +2302,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>201</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2240,7 +2311,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>202</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2249,7 +2320,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2257,7 +2328,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>204</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2265,7 +2336,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2273,7 +2344,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2281,7 +2352,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2289,7 +2360,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2297,7 +2368,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2305,7 +2376,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>210</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2313,7 +2384,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2321,7 +2392,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2332,7 +2403,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>213</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2340,7 +2411,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>214</v>
+        <v>224</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2348,7 +2419,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>215</v>
+        <v>225</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,7 +2427,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,7 +2435,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2372,7 +2443,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2380,7 +2451,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2388,7 +2459,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>220</v>
+        <v>230</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2396,7 +2467,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2404,7 +2475,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2444,7 +2515,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2452,7 +2523,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2460,7 +2531,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>225</v>
+        <v>235</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2476,7 +2547,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>226</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2484,7 +2555,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>227</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2492,7 +2563,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2500,7 +2571,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2508,7 +2579,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2516,7 +2587,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2524,18 +2595,18 @@
         <v>88</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>231</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>232</v>
+        <v>128</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked more on marquees
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="252">
   <si>
     <t xml:space="preserve">MAIN MENU</t>
   </si>
@@ -419,6 +419,18 @@
   </si>
   <si>
     <t xml:space="preserve">I don’t have enough Action Points!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">game.marquee.player_turn_n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player Turn %0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">game.marquee.enemy_turn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enemy Turn</t>
   </si>
   <si>
     <t xml:space="preserve">Tillbaka</t>
@@ -884,10 +896,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C66" activeCellId="0" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1421,6 +1433,22 @@
       </c>
       <c r="C63" s="1" t="s">
         <v>131</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B65" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1460,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1468,7 +1496,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1476,7 +1504,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,7 +1512,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1492,7 +1520,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1500,7 +1528,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1508,7 +1536,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1519,7 +1547,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1528,7 +1556,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1537,7 +1565,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1553,7 +1581,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1561,7 +1589,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1569,7 +1597,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1577,7 +1605,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1585,7 +1613,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1593,7 +1621,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,7 +1629,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1609,7 +1637,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1620,7 +1648,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1628,7 +1656,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1636,7 +1664,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1644,7 +1672,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1652,7 +1680,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1660,7 +1688,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1668,7 +1696,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1676,7 +1704,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1684,7 +1712,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,7 +1720,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1732,7 +1760,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,7 +1768,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,7 +1776,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,7 +1792,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1772,7 +1800,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1780,7 +1808,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1788,7 +1816,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1796,7 +1824,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1804,7 +1832,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1812,7 +1840,7 @@
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1823,7 +1851,7 @@
         <v>128</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1831,7 +1859,7 @@
         <v>130</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1853,8 +1881,8 @@
   </sheetPr>
   <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C46" activeCellId="0" sqref="C46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B47" activeCellId="0" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1872,7 +1900,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1880,7 +1908,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1888,7 +1916,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1896,7 +1924,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1904,7 +1932,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1912,7 +1940,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1920,7 +1948,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1931,7 +1959,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1940,7 +1968,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1949,7 +1977,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1965,7 +1993,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1973,7 +2001,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1981,7 +2009,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1989,7 +2017,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1997,7 +2025,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2005,7 +2033,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2013,7 +2041,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2021,7 +2049,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,7 +2060,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2040,7 +2068,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2048,7 +2076,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2056,7 +2084,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2072,7 +2100,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,7 +2108,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2088,7 +2116,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2096,7 +2124,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2104,7 +2132,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2144,7 +2172,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2180,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2160,7 +2188,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2176,7 +2204,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2184,7 +2212,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2192,7 +2220,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2200,7 +2228,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2208,7 +2236,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2216,7 +2244,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,7 +2252,7 @@
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2235,7 +2263,7 @@
         <v>128</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2243,7 +2271,7 @@
         <v>130</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2282,7 +2310,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2290,7 +2318,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2298,7 +2326,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2306,7 +2334,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2314,7 +2342,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2330,7 +2358,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2341,7 +2369,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2350,7 +2378,7 @@
         <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2359,7 +2387,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2367,7 +2395,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2375,7 +2403,7 @@
         <v>24</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2383,7 +2411,7 @@
         <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2391,7 +2419,7 @@
         <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2399,7 +2427,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2407,7 +2435,7 @@
         <v>32</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2415,7 +2443,7 @@
         <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2423,7 +2451,7 @@
         <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2431,7 +2459,7 @@
         <v>38</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2442,7 +2470,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2450,7 +2478,7 @@
         <v>43</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2458,7 +2486,7 @@
         <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2466,7 +2494,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,7 +2502,7 @@
         <v>49</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2482,7 +2510,7 @@
         <v>51</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2490,7 +2518,7 @@
         <v>53</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2498,7 +2526,7 @@
         <v>55</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2506,7 +2534,7 @@
         <v>57</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2514,7 +2542,7 @@
         <v>59</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2554,7 +2582,7 @@
         <v>69</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2562,7 +2590,7 @@
         <v>71</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2570,7 +2598,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2586,7 +2614,7 @@
         <v>77</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,7 +2622,7 @@
         <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2602,7 +2630,7 @@
         <v>81</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2610,7 +2638,7 @@
         <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2618,7 +2646,7 @@
         <v>84</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2626,7 +2654,7 @@
         <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2634,7 +2662,7 @@
         <v>88</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2645,15 +2673,15 @@
         <v>128</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C46" s="0" t="s">
-        <v>247</v>
+      <c r="C46" s="1" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added wishlist on Steam button
</commit_message>
<xml_diff>
--- a/game/ui-localizations.xlsx
+++ b/game/ui-localizations.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="258">
   <si>
     <t xml:space="preserve">MAIN MENU</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t xml:space="preserve">Quit Game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menu.wishlist_steam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wishlist us on Steam</t>
   </si>
   <si>
     <t xml:space="preserve">CHARACTER</t>
@@ -908,10 +914,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -980,18 +986,17 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1009,6 +1014,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>22</v>
       </c>
@@ -1076,26 +1082,26 @@
       <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="3" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="3" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1236,7 +1242,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="1" t="s">
         <v>79</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1256,15 +1262,15 @@
         <v>83</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1324,28 +1330,28 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="1" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="1" t="s">
         <v>106</v>
       </c>
@@ -1362,17 +1368,17 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="C54" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="1" t="s">
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="1" t="s">
         <v>113</v>
       </c>
@@ -1429,17 +1435,17 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B62" s="1" t="s">
+      <c r="C62" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C62" s="1" t="s">
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="1" t="s">
         <v>130</v>
       </c>
@@ -1467,7 +1473,7 @@
       <c r="B66" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="1" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1475,8 +1481,16 @@
       <c r="B67" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="1" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1516,7 +1530,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1524,7 +1538,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1532,7 +1546,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1540,7 +1554,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1548,7 +1562,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1556,7 +1570,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1564,330 +1578,330 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1928,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1936,7 +1950,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1944,7 +1958,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1952,7 +1966,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1960,7 +1974,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1968,7 +1982,7 @@
         <v>11</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1976,330 +1990,330 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2338,7 +2352,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2346,7 +2360,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2354,7 +2368,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2362,7 +2376,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2370,7 +2384,7 @@
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2386,330 +2400,330 @@
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3"/>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>